<commit_message>
Minor fix : Resetting ID column to 52 riverpoints
</commit_message>
<xml_diff>
--- a/Perseus-4.6_39rivers_mesh24.xlsx
+++ b/Perseus-4.6_39rivers_mesh24.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7360" yWindow="3440" windowWidth="34100" windowHeight="16740" tabRatio="992"/>
+    <workbookView xWindow="16280" yWindow="1980" windowWidth="34100" windowHeight="16740" tabRatio="992"/>
   </bookViews>
   <sheets>
     <sheet name="monthly" sheetId="1" r:id="rId1"/>
@@ -750,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2087,7 +2087,7 @@
     </row>
     <row r="21" spans="1:24">
       <c r="A21" s="1">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -2153,7 +2153,7 @@
     </row>
     <row r="22" spans="1:24">
       <c r="A22" s="1">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -2219,7 +2219,7 @@
     </row>
     <row r="23" spans="1:24">
       <c r="A23" s="1">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2285,7 +2285,7 @@
     </row>
     <row r="24" spans="1:24">
       <c r="A24" s="1">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -2351,7 +2351,7 @@
     </row>
     <row r="25" spans="1:24">
       <c r="A25" s="1">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2417,7 +2417,7 @@
     </row>
     <row r="26" spans="1:24">
       <c r="A26" s="1">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -2483,7 +2483,7 @@
     </row>
     <row r="27" spans="1:24">
       <c r="A27" s="1">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -2549,7 +2549,7 @@
     </row>
     <row r="28" spans="1:24">
       <c r="A28" s="1">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -2615,7 +2615,7 @@
     </row>
     <row r="29" spans="1:24">
       <c r="A29" s="1">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -2681,7 +2681,7 @@
     </row>
     <row r="30" spans="1:24">
       <c r="A30" s="1">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -2747,7 +2747,7 @@
     </row>
     <row r="31" spans="1:24">
       <c r="A31" s="1">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -2813,7 +2813,7 @@
     </row>
     <row r="32" spans="1:24">
       <c r="A32" s="1">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -2879,7 +2879,7 @@
     </row>
     <row r="33" spans="1:24">
       <c r="A33" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -2945,7 +2945,7 @@
     </row>
     <row r="34" spans="1:24">
       <c r="A34" s="1">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -3011,7 +3011,7 @@
     </row>
     <row r="35" spans="1:24">
       <c r="A35" s="1">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -3077,7 +3077,7 @@
     </row>
     <row r="36" spans="1:24">
       <c r="A36" s="1">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -3143,7 +3143,7 @@
     </row>
     <row r="37" spans="1:24">
       <c r="A37" s="1">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -3209,7 +3209,7 @@
     </row>
     <row r="38" spans="1:24">
       <c r="A38" s="1">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -3275,7 +3275,7 @@
     </row>
     <row r="39" spans="1:24">
       <c r="A39" s="1">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -3341,7 +3341,7 @@
     </row>
     <row r="40" spans="1:24">
       <c r="A40" s="1">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -3407,7 +3407,7 @@
     </row>
     <row r="41" spans="1:24">
       <c r="A41" s="1">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -3473,7 +3473,7 @@
     </row>
     <row r="42" spans="1:24">
       <c r="A42" s="1">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -3539,7 +3539,7 @@
     </row>
     <row r="43" spans="1:24">
       <c r="A43" s="1">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -3605,7 +3605,7 @@
     </row>
     <row r="44" spans="1:24">
       <c r="A44" s="1">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -3671,7 +3671,7 @@
     </row>
     <row r="45" spans="1:24">
       <c r="A45" s="1">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -3737,7 +3737,7 @@
     </row>
     <row r="46" spans="1:24">
       <c r="A46" s="1">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -3803,7 +3803,7 @@
     </row>
     <row r="47" spans="1:24">
       <c r="A47" s="1">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -3869,7 +3869,7 @@
     </row>
     <row r="48" spans="1:24">
       <c r="A48" s="1">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -3935,7 +3935,7 @@
     </row>
     <row r="49" spans="1:24">
       <c r="A49" s="1">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -4001,7 +4001,7 @@
     </row>
     <row r="50" spans="1:24">
       <c r="A50" s="1">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -4067,7 +4067,7 @@
     </row>
     <row r="51" spans="1:24">
       <c r="A51" s="1">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -4133,7 +4133,7 @@
     </row>
     <row r="52" spans="1:24">
       <c r="A52" s="1">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -4199,7 +4199,7 @@
     </row>
     <row r="53" spans="1:24">
       <c r="A53" s="1">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>

</xml_diff>